<commit_message>
Fix and sort Excel files
</commit_message>
<xml_diff>
--- a/COPsyncPresenceMap.WPF/COPsyncMaps/Alaska/Alaska.xlsx
+++ b/COPsyncPresenceMap.WPF/COPsyncMaps/Alaska/Alaska.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amoschini\Downloads\COPsyncMaps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amoschini\Documents\COPsyncMaps\Alaska\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>ElementId</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Yukon-Koyukuk</t>
+  </si>
+  <si>
+    <t>Anchorage</t>
+  </si>
+  <si>
+    <t>AK_Anchorage</t>
   </si>
 </sst>
 </file>
@@ -572,7 +578,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -623,198 +629,206 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>12</v>
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
+        <v>38</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>56</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="4"/>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="4"/>
     </row>
   </sheetData>
   <sortState ref="A2:E136">

</xml_diff>